<commit_message>
Stlye and hts logic fixes
</commit_message>
<xml_diff>
--- a/test_files/test1.xlsx
+++ b/test_files/test1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26926"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GitHub\Python Projects\Flask_new_project\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A29E141-CBB4-4FAB-ABBF-23DD271C2924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C6A9E3-C313-407D-85C6-CAF852CD4D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="150">
   <si>
     <t>ImporterAccount</t>
   </si>
@@ -482,6 +482,12 @@
   </si>
   <si>
     <t>8484.10.003300</t>
+  </si>
+  <si>
+    <t>super text long description of text in the event of a super teadsfasfewafaewgawegfawefewa long text</t>
+  </si>
+  <si>
+    <t>8484.00.00</t>
   </si>
 </sst>
 </file>
@@ -2835,7 +2841,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="82" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="82" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="652">
     <cellStyle name="_x0007_" xfId="71" xr:uid="{D802DB1D-7AE1-4193-8BDA-5E4EB46235C7}"/>
@@ -3793,8 +3799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH1194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4022,7 +4028,7 @@
       </c>
       <c r="AG4" s="10"/>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:34" ht="57">
       <c r="A5" t="s">
         <v>144</v>
       </c>
@@ -4033,7 +4039,7 @@
         <v>95</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>90</v>
@@ -5113,8 +5119,8 @@
       </c>
       <c r="F42" s="13"/>
       <c r="G42" s="20"/>
-      <c r="K42" s="32">
-        <v>84840000</v>
+      <c r="K42" s="32" t="s">
+        <v>149</v>
       </c>
       <c r="S42" s="17" t="s">
         <v>90</v>

</xml_diff>